<commit_message>
busfor, e-traffic, словарь городов, tutu, avtovokzal
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -16066,7 +16066,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16075,7 +16075,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" style="7" min="1" max="1"/>
-    <col width="9" customWidth="1" style="7" min="2" max="2"/>
+    <col width="14" customWidth="1" style="7" min="2" max="2"/>
     <col width="22" customWidth="1" style="7" min="3" max="3"/>
     <col width="21" customWidth="1" style="7" min="4" max="4"/>
     <col width="28" customWidth="1" style="7" min="5" max="5"/>
@@ -16083,7 +16083,7 @@
     <col width="12" customWidth="1" style="7" min="7" max="7"/>
     <col width="17" customWidth="1" style="7" min="8" max="8"/>
     <col width="32" customWidth="1" style="7" min="9" max="9"/>
-    <col width="11" customWidth="1" style="7" min="10" max="10"/>
+    <col width="15" customWidth="1" style="7" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -18214,10 +18214,8 @@
           <t>07:30</t>
         </is>
       </c>
-      <c r="B52" s="10" t="inlineStr">
-        <is>
-          <t>958</t>
-        </is>
+      <c r="B52" s="11" t="n">
+        <v>958</v>
       </c>
       <c r="C52" s="10" t="inlineStr">
         <is>
@@ -18239,16 +18237,8 @@
           <t>14</t>
         </is>
       </c>
-      <c r="G52" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H52" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="G52" s="10" t="inlineStr"/>
+      <c r="H52" s="10" t="inlineStr"/>
       <c r="I52" s="11" t="n">
         <v>890</v>
       </c>
@@ -18264,10 +18254,8 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B53" s="10" t="inlineStr">
-        <is>
-          <t>6694</t>
-        </is>
+      <c r="B53" s="11" t="n">
+        <v>6694</v>
       </c>
       <c r="C53" s="10" t="inlineStr">
         <is>
@@ -18289,15 +18277,11 @@
           <t>34</t>
         </is>
       </c>
-      <c r="G53" s="10" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
-      </c>
-      <c r="H53" s="10" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="G53" s="11" t="n">
+        <v>49</v>
+      </c>
+      <c r="H53" s="11" t="n">
+        <v>15</v>
       </c>
       <c r="I53" s="11" t="n">
         <v>620</v>
@@ -18314,10 +18298,8 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B54" s="10" t="inlineStr">
-        <is>
-          <t>3404</t>
-        </is>
+      <c r="B54" s="11" t="n">
+        <v>3404</v>
       </c>
       <c r="C54" s="10" t="inlineStr">
         <is>
@@ -18339,15 +18321,11 @@
           <t>21</t>
         </is>
       </c>
-      <c r="G54" s="10" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
-      </c>
-      <c r="H54" s="10" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="G54" s="11" t="n">
+        <v>49</v>
+      </c>
+      <c r="H54" s="11" t="n">
+        <v>28</v>
       </c>
       <c r="I54" s="11" t="n">
         <v>566</v>
@@ -18358,125 +18336,2131 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B55" s="10" t="inlineStr">
+        <is>
+          <t>109756900</t>
+        </is>
+      </c>
+      <c r="C55" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D55" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E55" s="10" t="inlineStr"/>
+      <c r="F55" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G55" s="10" t="inlineStr"/>
+      <c r="H55" s="10" t="inlineStr"/>
+      <c r="I55" s="11" t="n">
+        <v>4343.55</v>
+      </c>
+      <c r="J55" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B56" s="10" t="inlineStr">
+        <is>
+          <t>97647500</t>
+        </is>
+      </c>
+      <c r="C56" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D56" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E56" s="10" t="inlineStr"/>
+      <c r="F56" s="10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G56" s="10" t="inlineStr"/>
+      <c r="H56" s="10" t="inlineStr"/>
+      <c r="I56" s="11" t="n">
+        <v>3877.8</v>
+      </c>
+      <c r="J56" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
     <row r="57">
-      <c r="A57" s="12" t="inlineStr">
-        <is>
-          <t>Статистика</t>
-        </is>
-      </c>
-      <c r="B57" s="13" t="n"/>
+      <c r="A57" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B57" s="10" t="inlineStr">
+        <is>
+          <t>5406</t>
+        </is>
+      </c>
+      <c r="C57" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D57" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E57" s="10" t="inlineStr"/>
+      <c r="F57" s="10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G57" s="10" t="inlineStr"/>
+      <c r="H57" s="10" t="inlineStr"/>
+      <c r="I57" s="11" t="n">
+        <v>3296.48</v>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="10" t="inlineStr">
         <is>
-          <t>Всего рейсов</t>
-        </is>
-      </c>
-      <c r="B58" s="11" t="n">
-        <v>52</v>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B58" s="10" t="inlineStr">
+        <is>
+          <t>ЭКОЛАЙНС</t>
+        </is>
+      </c>
+      <c r="C58" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D58" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E58" s="10" t="inlineStr"/>
+      <c r="F58" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G58" s="10" t="inlineStr"/>
+      <c r="H58" s="10" t="inlineStr"/>
+      <c r="I58" s="11" t="n">
+        <v>4560.9</v>
+      </c>
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="10" t="inlineStr">
         <is>
-          <t>Средняя цена (руб.)</t>
-        </is>
-      </c>
-      <c r="B59" s="11" t="n">
-        <v>713.23</v>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B59" s="10" t="inlineStr">
+        <is>
+          <t>ЭКОЛАЙНС</t>
+        </is>
+      </c>
+      <c r="C59" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D59" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E59" s="10" t="inlineStr"/>
+      <c r="F59" s="10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G59" s="10" t="inlineStr"/>
+      <c r="H59" s="10" t="inlineStr"/>
+      <c r="I59" s="11" t="n">
+        <v>4072.15</v>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="12" t="inlineStr">
-        <is>
-          <t>Направления (Откуда)</t>
-        </is>
-      </c>
-      <c r="B60" s="13" t="n"/>
+      <c r="A60" s="10" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="B60" s="10" t="inlineStr">
+        <is>
+          <t>110477746</t>
+        </is>
+      </c>
+      <c r="C60" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D60" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E60" s="10" t="inlineStr"/>
+      <c r="F60" s="10" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="G60" s="10" t="inlineStr"/>
+      <c r="H60" s="10" t="inlineStr"/>
+      <c r="I60" s="11" t="n">
+        <v>3424.7</v>
+      </c>
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="B61" s="11" t="n">
-        <v>52</v>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="B61" s="10" t="inlineStr">
+        <is>
+          <t>8194</t>
+        </is>
+      </c>
+      <c r="C61" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D61" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E61" s="10" t="inlineStr"/>
+      <c r="F61" s="10" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="G61" s="10" t="inlineStr"/>
+      <c r="H61" s="10" t="inlineStr"/>
+      <c r="I61" s="11" t="n">
+        <v>2910.65</v>
+      </c>
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="12" t="inlineStr">
-        <is>
-          <t>Прибытие (Куда)</t>
-        </is>
-      </c>
-      <c r="B62" s="13" t="n"/>
+      <c r="A62" s="10" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="B62" s="10" t="inlineStr">
+        <is>
+          <t>Круиз</t>
+        </is>
+      </c>
+      <c r="C62" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D62" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E62" s="10" t="inlineStr"/>
+      <c r="F62" s="10" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="G62" s="10" t="inlineStr"/>
+      <c r="H62" s="10" t="inlineStr"/>
+      <c r="I62" s="11" t="n">
+        <v>3596.05</v>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Великий Новгород</t>
-        </is>
-      </c>
-      <c r="B63" s="11" t="n">
-        <v>52</v>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B63" s="10" t="inlineStr">
+        <is>
+          <t>110477747</t>
+        </is>
+      </c>
+      <c r="C63" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D63" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E63" s="10" t="inlineStr"/>
+      <c r="F63" s="10" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="G63" s="10" t="inlineStr"/>
+      <c r="H63" s="10" t="inlineStr"/>
+      <c r="I63" s="11" t="n">
+        <v>2847.4</v>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="12" t="inlineStr">
-        <is>
-          <t>Перевозчики</t>
-        </is>
-      </c>
-      <c r="B64" s="13" t="n"/>
+      <c r="A64" s="10" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B64" s="10" t="inlineStr">
+        <is>
+          <t>4571</t>
+        </is>
+      </c>
+      <c r="C64" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D64" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E64" s="10" t="inlineStr"/>
+      <c r="F64" s="10" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="G64" s="10" t="inlineStr"/>
+      <c r="H64" s="10" t="inlineStr"/>
+      <c r="I64" s="11" t="n">
+        <v>2420.51</v>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "СКСавто"</t>
-        </is>
-      </c>
-      <c r="B65" s="11" t="n">
-        <v>41</v>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B65" s="10" t="inlineStr">
+        <is>
+          <t>Беркут</t>
+        </is>
+      </c>
+      <c r="C65" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D65" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E65" s="10" t="inlineStr"/>
+      <c r="F65" s="10" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="G65" s="10" t="inlineStr"/>
+      <c r="H65" s="10" t="inlineStr"/>
+      <c r="I65" s="11" t="n">
+        <v>2990</v>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "ФАБУС"</t>
-        </is>
-      </c>
-      <c r="B66" s="11" t="n">
-        <v>7</v>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B66" s="10" t="inlineStr">
+        <is>
+          <t>103415422</t>
+        </is>
+      </c>
+      <c r="C66" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D66" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E66" s="10" t="inlineStr"/>
+      <c r="F66" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G66" s="10" t="inlineStr"/>
+      <c r="H66" s="10" t="inlineStr"/>
+      <c r="I66" s="11" t="n">
+        <v>3734.05</v>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО"Фабус"</t>
-        </is>
-      </c>
-      <c r="B67" s="11" t="n">
-        <v>2</v>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B67" s="10" t="inlineStr">
+        <is>
+          <t>104037811</t>
+        </is>
+      </c>
+      <c r="C67" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D67" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E67" s="10" t="inlineStr"/>
+      <c r="F67" s="10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G67" s="10" t="inlineStr"/>
+      <c r="H67" s="10" t="inlineStr"/>
+      <c r="I67" s="11" t="n">
+        <v>3111.9</v>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Яцунов Максим Сергеевич</t>
-        </is>
-      </c>
-      <c r="B68" s="11" t="n">
-        <v>1</v>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B68" s="10" t="inlineStr">
+        <is>
+          <t>110477748</t>
+        </is>
+      </c>
+      <c r="C68" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D68" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E68" s="10" t="inlineStr"/>
+      <c r="F68" s="10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G68" s="10" t="inlineStr"/>
+      <c r="H68" s="10" t="inlineStr"/>
+      <c r="I68" s="11" t="n">
+        <v>2995.75</v>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="10" t="inlineStr">
         <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B69" s="10" t="inlineStr">
+        <is>
+          <t>ТК</t>
+        </is>
+      </c>
+      <c r="C69" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D69" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E69" s="10" t="inlineStr"/>
+      <c r="F69" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G69" s="10" t="inlineStr"/>
+      <c r="H69" s="10" t="inlineStr"/>
+      <c r="I69" s="11" t="n">
+        <v>3174</v>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B70" s="10" t="inlineStr">
+        <is>
+          <t>ФТК</t>
+        </is>
+      </c>
+      <c r="C70" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D70" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E70" s="10" t="inlineStr"/>
+      <c r="F70" s="10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G70" s="10" t="inlineStr"/>
+      <c r="H70" s="10" t="inlineStr"/>
+      <c r="I70" s="11" t="n">
+        <v>2089.55</v>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B71" s="10" t="inlineStr">
+        <is>
+          <t>4359</t>
+        </is>
+      </c>
+      <c r="C71" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D71" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E71" s="10" t="inlineStr"/>
+      <c r="F71" s="10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G71" s="10" t="inlineStr"/>
+      <c r="H71" s="10" t="inlineStr"/>
+      <c r="I71" s="11" t="n">
+        <v>2545.86</v>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B72" s="10" t="inlineStr">
+        <is>
+          <t>78.77.031</t>
+        </is>
+      </c>
+      <c r="C72" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D72" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E72" s="10" t="inlineStr"/>
+      <c r="F72" s="10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G72" s="10" t="inlineStr"/>
+      <c r="H72" s="10" t="inlineStr"/>
+      <c r="I72" s="11" t="n">
+        <v>1723.85</v>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B73" s="10" t="inlineStr">
+        <is>
+          <t>r10939_23:00</t>
+        </is>
+      </c>
+      <c r="C73" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D73" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E73" s="10" t="inlineStr"/>
+      <c r="F73" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G73" s="10" t="inlineStr"/>
+      <c r="H73" s="10" t="inlineStr"/>
+      <c r="I73" s="11" t="n">
+        <v>2645</v>
+      </c>
+      <c r="J73" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B74" s="10" t="inlineStr">
+        <is>
+          <t>ВолгаЛинии</t>
+        </is>
+      </c>
+      <c r="C74" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D74" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E74" s="10" t="inlineStr"/>
+      <c r="F74" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G74" s="10" t="inlineStr"/>
+      <c r="H74" s="10" t="inlineStr"/>
+      <c r="I74" s="11" t="n">
+        <v>3920.35</v>
+      </c>
+      <c r="J74" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B75" s="10" t="inlineStr">
+        <is>
+          <t>ВолгаЛинии</t>
+        </is>
+      </c>
+      <c r="C75" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D75" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E75" s="10" t="inlineStr"/>
+      <c r="F75" s="10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G75" s="10" t="inlineStr"/>
+      <c r="H75" s="10" t="inlineStr"/>
+      <c r="I75" s="11" t="n">
+        <v>3267.15</v>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B76" s="10" t="inlineStr">
+        <is>
+          <t>ВолгаЛинии</t>
+        </is>
+      </c>
+      <c r="C76" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D76" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E76" s="10" t="inlineStr"/>
+      <c r="F76" s="10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G76" s="10" t="inlineStr"/>
+      <c r="H76" s="10" t="inlineStr"/>
+      <c r="I76" s="11" t="n">
+        <v>3145.25</v>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B77" s="10" t="inlineStr">
+        <is>
+          <t>109756900</t>
+        </is>
+      </c>
+      <c r="C77" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D77" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E77" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F77" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G77" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I77" s="11" t="n">
+        <v>4343.55</v>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B78" s="10" t="inlineStr">
+        <is>
+          <t>97647500</t>
+        </is>
+      </c>
+      <c r="C78" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D78" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E78" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F78" s="10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G78" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I78" s="11" t="n">
+        <v>3877.8</v>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B79" s="10" t="inlineStr">
+        <is>
+          <t>5406</t>
+        </is>
+      </c>
+      <c r="C79" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D79" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E79" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F79" s="10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G79" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I79" s="11" t="n">
+        <v>3296.48</v>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B80" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C80" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D80" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E80" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F80" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G80" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I80" s="11" t="n">
+        <v>4560.9</v>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B81" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C81" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D81" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E81" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F81" s="10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G81" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I81" s="11" t="n">
+        <v>4072.15</v>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="10" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="B82" s="10" t="inlineStr">
+        <is>
+          <t>110477746</t>
+        </is>
+      </c>
+      <c r="C82" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D82" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E82" s="10" t="inlineStr">
+        <is>
+          <t>Круиз 21</t>
+        </is>
+      </c>
+      <c r="F82" s="10" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="G82" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I82" s="11" t="n">
+        <v>3424.7</v>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="10" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="B83" s="10" t="inlineStr">
+        <is>
+          <t>8194</t>
+        </is>
+      </c>
+      <c r="C83" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D83" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E83" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Круиз 21"</t>
+        </is>
+      </c>
+      <c r="F83" s="10" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="G83" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I83" s="11" t="n">
+        <v>2910.65</v>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="10" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="B84" s="10" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C84" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D84" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E84" s="10" t="inlineStr">
+        <is>
+          <t>Круиз 21</t>
+        </is>
+      </c>
+      <c r="F84" s="10" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="G84" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I84" s="11" t="n">
+        <v>3596.05</v>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="10" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B85" s="10" t="inlineStr">
+        <is>
+          <t>110477747</t>
+        </is>
+      </c>
+      <c r="C85" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D85" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E85" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F85" s="10" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="G85" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I85" s="11" t="n">
+        <v>2847.4</v>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="10" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B86" s="10" t="inlineStr">
+        <is>
+          <t>4571</t>
+        </is>
+      </c>
+      <c r="C86" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D86" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E86" s="10" t="inlineStr">
+        <is>
+          <t>ООО "БЕРКУТ"</t>
+        </is>
+      </c>
+      <c r="F86" s="10" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="G86" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I86" s="11" t="n">
+        <v>2420.51</v>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="10" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B87" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C87" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D87" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E87" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F87" s="10" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="G87" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I87" s="11" t="n">
+        <v>2990</v>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B88" s="10" t="inlineStr">
+        <is>
+          <t>103415422</t>
+        </is>
+      </c>
+      <c r="C88" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D88" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E88" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F88" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G88" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I88" s="11" t="n">
+        <v>3734.05</v>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B89" s="10" t="inlineStr">
+        <is>
+          <t>104037811</t>
+        </is>
+      </c>
+      <c r="C89" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D89" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E89" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F89" s="10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G89" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I89" s="11" t="n">
+        <v>3111.9</v>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B90" s="10" t="inlineStr">
+        <is>
+          <t>110477748</t>
+        </is>
+      </c>
+      <c r="C90" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D90" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E90" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F90" s="10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G90" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I90" s="11" t="n">
+        <v>2995.75</v>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B91" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C91" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D91" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E91" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F91" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G91" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I91" s="11" t="n">
+        <v>3174</v>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B92" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C92" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D92" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E92" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F92" s="10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G92" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I92" s="11" t="n">
+        <v>2089.55</v>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B93" s="10" t="inlineStr">
+        <is>
+          <t>4359</t>
+        </is>
+      </c>
+      <c r="C93" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D93" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E93" s="10" t="inlineStr">
+        <is>
+          <t>ООО "ВОЛГАЛИНИИ"</t>
+        </is>
+      </c>
+      <c r="F93" s="10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G93" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I93" s="11" t="n">
+        <v>2545.86</v>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B94" s="10" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="C94" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D94" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E94" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F94" s="10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G94" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H94" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I94" s="11" t="n">
+        <v>1723.85</v>
+      </c>
+      <c r="J94" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B95" s="10" t="inlineStr">
+        <is>
+          <t>10939</t>
+        </is>
+      </c>
+      <c r="C95" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D95" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E95" s="10" t="inlineStr">
+        <is>
+          <t>ООО "ВОЛГАЛИНИИ"</t>
+        </is>
+      </c>
+      <c r="F95" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G95" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H95" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I95" s="11" t="n">
+        <v>2645</v>
+      </c>
+      <c r="J95" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B96" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C96" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D96" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E96" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F96" s="10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G96" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H96" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I96" s="11" t="n">
+        <v>3920.35</v>
+      </c>
+      <c r="J96" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B97" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C97" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D97" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E97" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F97" s="10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G97" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H97" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I97" s="11" t="n">
+        <v>3267.15</v>
+      </c>
+      <c r="J97" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B98" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C98" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D98" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E98" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F98" s="10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G98" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H98" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I98" s="11" t="n">
+        <v>3145.25</v>
+      </c>
+      <c r="J98" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="12" t="inlineStr">
+        <is>
+          <t>Статистика</t>
+        </is>
+      </c>
+      <c r="B101" s="13" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="10" t="inlineStr">
+        <is>
+          <t>Всего рейсов</t>
+        </is>
+      </c>
+      <c r="B102" s="11" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="10" t="inlineStr">
+        <is>
+          <t>Средняя цена (руб.)</t>
+        </is>
+      </c>
+      <c r="B103" s="11" t="n">
+        <v>1859.1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="12" t="inlineStr">
+        <is>
+          <t>Направления (Откуда)</t>
+        </is>
+      </c>
+      <c r="B104" s="13" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="B105" s="11" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="12" t="inlineStr">
+        <is>
+          <t>Прибытие (Куда)</t>
+        </is>
+      </c>
+      <c r="B106" s="13" t="n"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Великий Новгород</t>
+        </is>
+      </c>
+      <c r="B107" s="11" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Москва</t>
+        </is>
+      </c>
+      <c r="B108" s="11" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="12" t="inlineStr">
+        <is>
+          <t>Перевозчики</t>
+        </is>
+      </c>
+      <c r="B109" s="13" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "СКСавто"</t>
+        </is>
+      </c>
+      <c r="B110" s="11" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  N/A</t>
+        </is>
+      </c>
+      <c r="B111" s="11" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "ФАБУС"</t>
+        </is>
+      </c>
+      <c r="B112" s="11" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО"Фабус"</t>
+        </is>
+      </c>
+      <c r="B113" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Круиз 21</t>
+        </is>
+      </c>
+      <c r="B114" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="B115" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "ВОЛГАЛИНИИ"</t>
+        </is>
+      </c>
+      <c r="B116" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Яцунов Максим Сергеевич</t>
+        </is>
+      </c>
+      <c r="B117" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="10" t="inlineStr">
+        <is>
           <t xml:space="preserve">  СКСавто</t>
         </is>
       </c>
-      <c r="B69" s="11" t="n">
+      <c r="B118" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "Круиз 21"</t>
+        </is>
+      </c>
+      <c r="B119" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "БЕРКУТ"</t>
+        </is>
+      </c>
+      <c r="B120" s="11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
busfor, e-traffic, словарь городов, tutu, avtovokzal, render2
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -15,6 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-08-08" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-08-07" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-08-11" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-08-12" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -4391,6 +4392,1577 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="34" customWidth="1" style="7" min="1" max="1"/>
+    <col width="11" customWidth="1" style="7" min="2" max="2"/>
+    <col width="22" customWidth="1" style="7" min="3" max="3"/>
+    <col width="21" customWidth="1" style="7" min="4" max="4"/>
+    <col width="32" customWidth="1" style="7" min="5" max="5"/>
+    <col width="12" customWidth="1" style="7" min="6" max="6"/>
+    <col width="15" customWidth="1" style="7" min="7" max="7"/>
+    <col width="17" customWidth="1" style="7" min="8" max="8"/>
+    <col width="32" customWidth="1" style="7" min="9" max="9"/>
+    <col width="15" customWidth="1" style="7" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Маршрут</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>Время отправления рейса с НП</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>№ рейса</t>
+        </is>
+      </c>
+      <c r="C2" s="9" t="inlineStr">
+        <is>
+          <t>НП - начальный пункт</t>
+        </is>
+      </c>
+      <c r="D2" s="9" t="inlineStr">
+        <is>
+          <t>КП - конечный пункт</t>
+        </is>
+      </c>
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>Перевозчик</t>
+        </is>
+      </c>
+      <c r="F2" s="9" t="inlineStr">
+        <is>
+          <t>Всего мест</t>
+        </is>
+      </c>
+      <c r="G2" s="9" t="inlineStr">
+        <is>
+          <t>Свободно мест</t>
+        </is>
+      </c>
+      <c r="H2" s="9" t="inlineStr">
+        <is>
+          <t>Продано билетов</t>
+        </is>
+      </c>
+      <c r="I2" s="9" t="inlineStr">
+        <is>
+          <t>Средняя цена за билет на рейсе</t>
+        </is>
+      </c>
+      <c r="J2" s="9" t="inlineStr">
+        <is>
+          <t>Источник</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="inlineStr">
+        <is>
+          <t>ООО "АСТОРИЯ"</t>
+        </is>
+      </c>
+      <c r="F3" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G3" s="10" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H3" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I3" s="11" t="n">
+        <v>9662.299999999999</v>
+      </c>
+      <c r="J3" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>106417595</t>
+        </is>
+      </c>
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H4" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" s="11" t="n">
+        <v>6765.45</v>
+      </c>
+      <c r="J4" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="inlineStr">
+        <is>
+          <t>106445121</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F5" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" s="11" t="n">
+        <v>5750</v>
+      </c>
+      <c r="J5" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H6" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>6969</v>
+      </c>
+      <c r="J6" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C7" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F7" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G7" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H7" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>6037.5</v>
+      </c>
+      <c r="J7" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H8" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>7103.55</v>
+      </c>
+      <c r="J8" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B9" s="10" t="inlineStr">
+        <is>
+          <t>94966603</t>
+        </is>
+      </c>
+      <c r="C9" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D9" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Д.С.</t>
+        </is>
+      </c>
+      <c r="F9" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G9" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>41401.15</v>
+      </c>
+      <c r="J9" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>98476309</t>
+        </is>
+      </c>
+      <c r="C10" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Д.С.</t>
+        </is>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>41401.15</v>
+      </c>
+      <c r="J10" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Дмитрий Сергеевич</t>
+        </is>
+      </c>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I11" s="11" t="n">
+        <v>35190</v>
+      </c>
+      <c r="J11" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>111614972</t>
+        </is>
+      </c>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I12" s="11" t="n">
+        <v>8117.85</v>
+      </c>
+      <c r="J12" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>111614973</t>
+        </is>
+      </c>
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F13" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G13" s="10" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I13" s="11" t="n">
+        <v>8117.85</v>
+      </c>
+      <c r="J13" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Елена Владимировна</t>
+        </is>
+      </c>
+      <c r="F14" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I14" s="11" t="n">
+        <v>6900</v>
+      </c>
+      <c r="J14" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Елена Владимировна</t>
+        </is>
+      </c>
+      <c r="F15" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G15" s="10" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I15" s="11" t="n">
+        <v>6900</v>
+      </c>
+      <c r="J15" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F16" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G16" s="10" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I16" s="11" t="n">
+        <v>8523.799999999999</v>
+      </c>
+      <c r="J16" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F17" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G17" s="10" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I17" s="11" t="n">
+        <v>8523.799999999999</v>
+      </c>
+      <c r="J17" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C18" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="inlineStr">
+        <is>
+          <t>ИП Насиров Махир Музаффар Оглы</t>
+        </is>
+      </c>
+      <c r="F18" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G18" s="10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I18" s="11" t="n">
+        <v>15994.2</v>
+      </c>
+      <c r="J18" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C19" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D19" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E19" s="10" t="inlineStr">
+        <is>
+          <t>ИП Насиров М.М.</t>
+        </is>
+      </c>
+      <c r="F19" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G19" s="10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I19" s="11" t="n">
+        <v>14614.2</v>
+      </c>
+      <c r="J19" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E20" s="10" t="inlineStr">
+        <is>
+          <t>ИП Насиров М.М.</t>
+        </is>
+      </c>
+      <c r="F20" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G20" s="10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I20" s="11" t="n">
+        <v>15166.2</v>
+      </c>
+      <c r="J20" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>105385976</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D21" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E21" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F21" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G21" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I21" s="11" t="n">
+        <v>6900</v>
+      </c>
+      <c r="J21" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>105391214</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D22" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E22" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F22" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G22" s="10" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I22" s="11" t="n">
+        <v>6900</v>
+      </c>
+      <c r="J22" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>106417597</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D23" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E23" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F23" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G23" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I23" s="11" t="n">
+        <v>8117.85</v>
+      </c>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>107998959</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D24" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E24" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F24" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G24" s="10" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I24" s="11" t="n">
+        <v>6900</v>
+      </c>
+      <c r="J24" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C25" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D25" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E25" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F25" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G25" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I25" s="11" t="n">
+        <v>8523.799999999999</v>
+      </c>
+      <c r="J25" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D26" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E26" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F26" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G26" s="10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I26" s="11" t="n">
+        <v>7245</v>
+      </c>
+      <c r="J26" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C27" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D27" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E27" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F27" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" s="10" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="H27" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I27" s="11" t="n">
+        <v>7245</v>
+      </c>
+      <c r="J27" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D28" s="10" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="E28" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F28" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G28" s="10" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H28" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I28" s="11" t="n">
+        <v>7245</v>
+      </c>
+      <c r="J28" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="12" t="inlineStr">
+        <is>
+          <t>Статистика</t>
+        </is>
+      </c>
+      <c r="B31" s="13" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="10" t="inlineStr">
+        <is>
+          <t>Всего рейсов</t>
+        </is>
+      </c>
+      <c r="B32" s="11" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="inlineStr">
+        <is>
+          <t>Средняя цена (руб.)</t>
+        </is>
+      </c>
+      <c r="B33" s="11" t="n">
+        <v>12008.26</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="12" t="inlineStr">
+        <is>
+          <t>Направления (Откуда)</t>
+        </is>
+      </c>
+      <c r="B34" s="13" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="12" t="inlineStr">
+        <is>
+          <t>Прибытие (Куда)</t>
+        </is>
+      </c>
+      <c r="B36" s="13" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="B37" s="11" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="12" t="inlineStr">
+        <is>
+          <t>Перевозчики</t>
+        </is>
+      </c>
+      <c r="B38" s="13" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="B39" s="11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="B40" s="11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="B41" s="11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Панин Д.С.</t>
+        </is>
+      </c>
+      <c r="B42" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Асеева Елена Владимировна</t>
+        </is>
+      </c>
+      <c r="B43" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Насиров М.М.</t>
+        </is>
+      </c>
+      <c r="B44" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "АСТОРИЯ"</t>
+        </is>
+      </c>
+      <c r="B45" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="B46" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Панин Дмитрий Сергеевич</t>
+        </is>
+      </c>
+      <c r="B47" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Насиров Махир Музаффар Оглы</t>
+        </is>
+      </c>
+      <c r="B48" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
busfor, e-traffic, словарь городов, tutu, avtovokzal, pandas
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -12560,7 +12560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12568,342 +12568,736 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" style="7" min="1" max="1"/>
-    <col width="9" customWidth="1" style="7" min="2" max="2"/>
-    <col width="22" customWidth="1" style="7" min="3" max="3"/>
-    <col width="21" customWidth="1" style="7" min="4" max="4"/>
+    <col width="50" customWidth="1" style="7" min="1" max="1"/>
+    <col width="11" customWidth="1" style="7" min="2" max="2"/>
+    <col width="48" customWidth="1" style="7" min="3" max="3"/>
+    <col width="28" customWidth="1" style="7" min="4" max="4"/>
     <col width="17" customWidth="1" style="7" min="5" max="5"/>
     <col width="15" customWidth="1" style="7" min="6" max="6"/>
     <col width="12" customWidth="1" style="7" min="7" max="7"/>
     <col width="17" customWidth="1" style="7" min="8" max="8"/>
     <col width="32" customWidth="1" style="7" min="9" max="9"/>
-    <col width="10" customWidth="1" style="7" min="10" max="10"/>
+    <col width="15" customWidth="1" style="7" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Маршрут</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>2025-08-13</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Время отправления рейса с НП</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="9" t="inlineStr">
         <is>
           <t>№ рейса</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="9" t="inlineStr">
         <is>
           <t>НП - начальный пункт</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="D2" s="9" t="inlineStr">
         <is>
           <t>КП - конечный пункт</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" s="9" t="inlineStr">
         <is>
           <t>Перевозчик</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" s="9" t="inlineStr">
         <is>
           <t>Свободно мест</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>Всего мест</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="H2" s="9" t="inlineStr">
         <is>
           <t>Продано билетов</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="I2" s="9" t="inlineStr">
         <is>
           <t>Средняя цена за билет на рейсе</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="J2" s="9" t="inlineStr">
         <is>
           <t>Источник</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="11" t="n">
         <v>856</v>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
         <is>
           <t>Кириши</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="10" t="inlineStr">
         <is>
           <t>ФТК Сотранс ООО</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="3" t="n">
+      <c r="G3" s="10" t="inlineStr"/>
+      <c r="H3" s="11" t="n">
         <v>40</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="11" t="n">
         <v>500</v>
       </c>
-      <c r="J3" s="2" t="inlineStr">
+      <c r="J3" s="10" t="inlineStr">
         <is>
           <t>busfor</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>18:50</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="11" t="n">
         <v>856</v>
       </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
         <is>
           <t>Кириши</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" s="10" t="inlineStr">
         <is>
           <t>ФТК Сотранс ООО</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="3" t="n">
+      <c r="G4" s="10" t="inlineStr"/>
+      <c r="H4" s="11" t="n">
         <v>40</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="11" t="n">
         <v>500</v>
       </c>
-      <c r="J4" s="2" t="inlineStr">
+      <c r="J4" s="10" t="inlineStr">
         <is>
           <t>busfor</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="11" t="n">
+        <v>856</v>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>Кириши</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F5" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr"/>
+      <c r="H5" s="11" t="n">
+        <v>40</v>
+      </c>
+      <c r="I5" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="J5" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>18:50</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>856</v>
+      </c>
+      <c r="C6" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>Кириши</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr"/>
+      <c r="H6" s="11" t="n">
+        <v>40</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="J6" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr"/>
+      <c r="C7" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, ост. Станция метро Волковская</t>
+        </is>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>Кириши, ост. Вокзал Кириши</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F7" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="G7" s="10" t="inlineStr"/>
+      <c r="H7" s="10" t="inlineStr"/>
+      <c r="I7" s="11" t="n">
+        <v>601</v>
+      </c>
+      <c r="J7" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr"/>
+      <c r="C8" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, ост. Станция метро Волковская</t>
+        </is>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>Кириши, ост. Вокзал Кириши</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr"/>
+      <c r="H8" s="10" t="inlineStr"/>
+      <c r="I8" s="11" t="n">
+        <v>601</v>
+      </c>
+      <c r="J8" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="B9" s="10" t="inlineStr">
+        <is>
+          <t>116327376</t>
+        </is>
+      </c>
+      <c r="C9" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D9" s="10" t="inlineStr">
+        <is>
+          <t>Кириши</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F9" s="10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="G9" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>676.2</v>
+      </c>
+      <c r="J9" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>116459708</t>
+        </is>
+      </c>
+      <c r="C10" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>Кириши</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>575</v>
+      </c>
+      <c r="J10" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
         <is>
           <t>856</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>Кириши</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E11" s="10" t="inlineStr">
         <is>
           <t>ФТК Сотранс ООО</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>10+</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>500</v>
-      </c>
-      <c r="J5" s="2" t="inlineStr">
-        <is>
-          <t>busfor</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>18:50</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I11" s="11" t="n">
+        <v>575</v>
+      </c>
+      <c r="J11" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>116327377</t>
+        </is>
+      </c>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>Кириши</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I12" s="11" t="n">
+        <v>676.2</v>
+      </c>
+      <c r="J12" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>116459709</t>
+        </is>
+      </c>
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>Кириши</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F13" s="10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="G13" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I13" s="11" t="n">
+        <v>575</v>
+      </c>
+      <c r="J13" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
         <is>
           <t>856</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>Кириши</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
+      <c r="E14" s="10" t="inlineStr">
         <is>
           <t>ФТК Сотранс ООО</t>
         </is>
       </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>10+</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>500</v>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>busfor</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="F14" s="10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I14" s="11" t="n">
+        <v>575</v>
+      </c>
+      <c r="J14" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12" t="inlineStr">
         <is>
           <t>Статистика</t>
         </is>
       </c>
-      <c r="B9" s="5" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="B17" s="13" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>Всего рейсов</t>
         </is>
       </c>
-      <c r="B10" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="B18" s="11" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>Средняя цена (руб.)</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="B19" s="11" t="n">
+        <v>571.2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="12" t="inlineStr">
         <is>
           <t>Направления (Откуда)</t>
         </is>
       </c>
-      <c r="B12" s="5" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="B20" s="13" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">  Санкт-Петербург</t>
         </is>
       </c>
-      <c r="B13" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="inlineStr">
+      <c r="B21" s="11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Санкт-Петербург, ост. Станция метро Волковская</t>
+        </is>
+      </c>
+      <c r="B22" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12" t="inlineStr">
         <is>
           <t>Прибытие (Куда)</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="B23" s="13" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">  Кириши</t>
         </is>
       </c>
-      <c r="B15" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="B24" s="11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Кириши, ост. Вокзал Кириши</t>
+        </is>
+      </c>
+      <c r="B25" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="12" t="inlineStr">
         <is>
           <t>Перевозчики</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="B26" s="13" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">  ФТК Сотранс ООО</t>
         </is>
       </c>
-      <c r="B17" s="3" t="n">
-        <v>4</v>
+      <c r="B27" s="11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="B28" s="11" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
busfor, e-traffic, словарь городов, tutu, avtovokzal, selenium
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -4398,7 +4398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4406,10 +4406,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="34" customWidth="1" style="7" min="1" max="1"/>
+    <col width="30" customWidth="1" style="7" min="1" max="1"/>
     <col width="11" customWidth="1" style="7" min="2" max="2"/>
-    <col width="22" customWidth="1" style="7" min="3" max="3"/>
-    <col width="21" customWidth="1" style="7" min="4" max="4"/>
+    <col width="41" customWidth="1" style="7" min="3" max="3"/>
+    <col width="50" customWidth="1" style="7" min="4" max="4"/>
     <col width="32" customWidth="1" style="7" min="5" max="5"/>
     <col width="12" customWidth="1" style="7" min="6" max="6"/>
     <col width="15" customWidth="1" style="7" min="7" max="7"/>
@@ -4488,11 +4488,7 @@
           <t>10:00</t>
         </is>
       </c>
-      <c r="B3" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B3" s="10" t="inlineStr"/>
       <c r="C3" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -4508,21 +4504,11 @@
           <t>ООО "АСТОРИЯ"</t>
         </is>
       </c>
-      <c r="F3" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G3" s="10" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H3" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F3" s="10" t="inlineStr"/>
+      <c r="G3" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H3" s="10" t="inlineStr"/>
       <c r="I3" s="11" t="n">
         <v>9662.299999999999</v>
       </c>
@@ -4538,10 +4524,8 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
-        <is>
-          <t>106417595</t>
-        </is>
+      <c r="B4" s="11" t="n">
+        <v>106417595</v>
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
@@ -4558,21 +4542,11 @@
           <t>ФТК Сотранс</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G4" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H4" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F4" s="10" t="inlineStr"/>
+      <c r="G4" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H4" s="10" t="inlineStr"/>
       <c r="I4" s="11" t="n">
         <v>6765.45</v>
       </c>
@@ -4588,10 +4562,8 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B5" s="10" t="inlineStr">
-        <is>
-          <t>106445121</t>
-        </is>
+      <c r="B5" s="11" t="n">
+        <v>106445121</v>
       </c>
       <c r="C5" s="10" t="inlineStr">
         <is>
@@ -4608,21 +4580,11 @@
           <t>ФТК Сотранс</t>
         </is>
       </c>
-      <c r="F5" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G5" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H5" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F5" s="10" t="inlineStr"/>
+      <c r="G5" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H5" s="10" t="inlineStr"/>
       <c r="I5" s="11" t="n">
         <v>5750</v>
       </c>
@@ -4638,11 +4600,7 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B6" s="10" t="inlineStr"/>
       <c r="C6" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -4658,21 +4616,11 @@
           <t>ФТК Сотранс ООО</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G6" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H6" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F6" s="10" t="inlineStr"/>
+      <c r="G6" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H6" s="10" t="inlineStr"/>
       <c r="I6" s="11" t="n">
         <v>6969</v>
       </c>
@@ -4688,11 +4636,7 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B7" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B7" s="10" t="inlineStr"/>
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -4708,21 +4652,11 @@
           <t>ФТК Сотранс</t>
         </is>
       </c>
-      <c r="F7" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G7" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H7" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F7" s="10" t="inlineStr"/>
+      <c r="G7" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H7" s="10" t="inlineStr"/>
       <c r="I7" s="11" t="n">
         <v>6037.5</v>
       </c>
@@ -4738,11 +4672,7 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B8" s="10" t="inlineStr"/>
       <c r="C8" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -4758,21 +4688,11 @@
           <t>ФТК Сотранс</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G8" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H8" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F8" s="10" t="inlineStr"/>
+      <c r="G8" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H8" s="10" t="inlineStr"/>
       <c r="I8" s="11" t="n">
         <v>7103.55</v>
       </c>
@@ -4788,10 +4708,8 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B9" s="10" t="inlineStr">
-        <is>
-          <t>94966603</t>
-        </is>
+      <c r="B9" s="11" t="n">
+        <v>94966603</v>
       </c>
       <c r="C9" s="10" t="inlineStr">
         <is>
@@ -4808,21 +4726,11 @@
           <t>ИП Панин Д.С.</t>
         </is>
       </c>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G9" s="10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="H9" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F9" s="10" t="inlineStr"/>
+      <c r="G9" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" s="10" t="inlineStr"/>
       <c r="I9" s="11" t="n">
         <v>41401.15</v>
       </c>
@@ -4838,10 +4746,8 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
-        <is>
-          <t>98476309</t>
-        </is>
+      <c r="B10" s="11" t="n">
+        <v>98476309</v>
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
@@ -4858,21 +4764,11 @@
           <t>ИП Панин Д.С.</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G10" s="10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F10" s="10" t="inlineStr"/>
+      <c r="G10" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="H10" s="10" t="inlineStr"/>
       <c r="I10" s="11" t="n">
         <v>41401.15</v>
       </c>
@@ -4888,11 +4784,7 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B11" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B11" s="10" t="inlineStr"/>
       <c r="C11" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -4908,21 +4800,11 @@
           <t>ИП Панин Дмитрий Сергеевич</t>
         </is>
       </c>
-      <c r="F11" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G11" s="10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F11" s="10" t="inlineStr"/>
+      <c r="G11" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" s="10" t="inlineStr"/>
       <c r="I11" s="11" t="n">
         <v>35190</v>
       </c>
@@ -4938,10 +4820,8 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
-        <is>
-          <t>111614972</t>
-        </is>
+      <c r="B12" s="11" t="n">
+        <v>111614972</v>
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
@@ -4958,21 +4838,11 @@
           <t>ИП Асеева Е.В.</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G12" s="10" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H12" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F12" s="10" t="inlineStr"/>
+      <c r="G12" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="H12" s="10" t="inlineStr"/>
       <c r="I12" s="11" t="n">
         <v>8117.85</v>
       </c>
@@ -4988,10 +4858,8 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B13" s="10" t="inlineStr">
-        <is>
-          <t>111614973</t>
-        </is>
+      <c r="B13" s="11" t="n">
+        <v>111614973</v>
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
@@ -5008,21 +4876,11 @@
           <t>ИП Асеева Е.В.</t>
         </is>
       </c>
-      <c r="F13" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G13" s="10" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H13" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F13" s="10" t="inlineStr"/>
+      <c r="G13" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="H13" s="10" t="inlineStr"/>
       <c r="I13" s="11" t="n">
         <v>8117.85</v>
       </c>
@@ -5038,11 +4896,7 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B14" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B14" s="10" t="inlineStr"/>
       <c r="C14" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5058,21 +4912,11 @@
           <t>ИП Асеева Елена Владимировна</t>
         </is>
       </c>
-      <c r="F14" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G14" s="10" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="H14" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F14" s="10" t="inlineStr"/>
+      <c r="G14" s="11" t="n">
+        <v>42</v>
+      </c>
+      <c r="H14" s="10" t="inlineStr"/>
       <c r="I14" s="11" t="n">
         <v>6900</v>
       </c>
@@ -5088,11 +4932,7 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B15" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B15" s="10" t="inlineStr"/>
       <c r="C15" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5108,21 +4948,11 @@
           <t>ИП Асеева Елена Владимировна</t>
         </is>
       </c>
-      <c r="F15" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G15" s="10" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="H15" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F15" s="10" t="inlineStr"/>
+      <c r="G15" s="11" t="n">
+        <v>42</v>
+      </c>
+      <c r="H15" s="10" t="inlineStr"/>
       <c r="I15" s="11" t="n">
         <v>6900</v>
       </c>
@@ -5138,11 +4968,7 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B16" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B16" s="10" t="inlineStr"/>
       <c r="C16" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5158,21 +4984,11 @@
           <t>ИП Асеева Е.В.</t>
         </is>
       </c>
-      <c r="F16" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G16" s="10" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H16" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F16" s="10" t="inlineStr"/>
+      <c r="G16" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="H16" s="10" t="inlineStr"/>
       <c r="I16" s="11" t="n">
         <v>8523.799999999999</v>
       </c>
@@ -5188,11 +5004,7 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B17" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B17" s="10" t="inlineStr"/>
       <c r="C17" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5208,21 +5020,11 @@
           <t>ИП Асеева Е.В.</t>
         </is>
       </c>
-      <c r="F17" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G17" s="10" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H17" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F17" s="10" t="inlineStr"/>
+      <c r="G17" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="H17" s="10" t="inlineStr"/>
       <c r="I17" s="11" t="n">
         <v>8523.799999999999</v>
       </c>
@@ -5238,11 +5040,7 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B18" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B18" s="10" t="inlineStr"/>
       <c r="C18" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5258,21 +5056,11 @@
           <t>ИП Насиров Махир Музаффар Оглы</t>
         </is>
       </c>
-      <c r="F18" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G18" s="10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H18" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F18" s="10" t="inlineStr"/>
+      <c r="G18" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H18" s="10" t="inlineStr"/>
       <c r="I18" s="11" t="n">
         <v>15994.2</v>
       </c>
@@ -5288,11 +5076,7 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B19" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B19" s="10" t="inlineStr"/>
       <c r="C19" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5308,21 +5092,11 @@
           <t>ИП Насиров М.М.</t>
         </is>
       </c>
-      <c r="F19" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G19" s="10" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H19" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F19" s="10" t="inlineStr"/>
+      <c r="G19" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H19" s="10" t="inlineStr"/>
       <c r="I19" s="11" t="n">
         <v>14614.2</v>
       </c>
@@ -5338,11 +5112,7 @@
           <t>21:00</t>
         </is>
       </c>
-      <c r="B20" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B20" s="10" t="inlineStr"/>
       <c r="C20" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5358,21 +5128,11 @@
           <t>ИП Насиров М.М.</t>
         </is>
       </c>
-      <c r="F20" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G20" s="10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H20" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F20" s="10" t="inlineStr"/>
+      <c r="G20" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="10" t="inlineStr"/>
       <c r="I20" s="11" t="n">
         <v>15166.2</v>
       </c>
@@ -5388,10 +5148,8 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B21" s="10" t="inlineStr">
-        <is>
-          <t>105385976</t>
-        </is>
+      <c r="B21" s="11" t="n">
+        <v>105385976</v>
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
@@ -5408,21 +5166,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F21" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G21" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H21" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F21" s="10" t="inlineStr"/>
+      <c r="G21" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H21" s="10" t="inlineStr"/>
       <c r="I21" s="11" t="n">
         <v>6900</v>
       </c>
@@ -5438,10 +5186,8 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B22" s="10" t="inlineStr">
-        <is>
-          <t>105391214</t>
-        </is>
+      <c r="B22" s="11" t="n">
+        <v>105391214</v>
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
@@ -5458,21 +5204,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F22" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G22" s="10" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="H22" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F22" s="10" t="inlineStr"/>
+      <c r="G22" s="11" t="n">
+        <v>31</v>
+      </c>
+      <c r="H22" s="10" t="inlineStr"/>
       <c r="I22" s="11" t="n">
         <v>6900</v>
       </c>
@@ -5488,10 +5224,8 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B23" s="10" t="inlineStr">
-        <is>
-          <t>106417597</t>
-        </is>
+      <c r="B23" s="11" t="n">
+        <v>106417597</v>
       </c>
       <c r="C23" s="10" t="inlineStr">
         <is>
@@ -5508,21 +5242,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F23" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G23" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H23" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F23" s="10" t="inlineStr"/>
+      <c r="G23" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H23" s="10" t="inlineStr"/>
       <c r="I23" s="11" t="n">
         <v>8117.85</v>
       </c>
@@ -5538,10 +5262,8 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B24" s="10" t="inlineStr">
-        <is>
-          <t>107998959</t>
-        </is>
+      <c r="B24" s="11" t="n">
+        <v>107998959</v>
       </c>
       <c r="C24" s="10" t="inlineStr">
         <is>
@@ -5558,21 +5280,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F24" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G24" s="10" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H24" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F24" s="10" t="inlineStr"/>
+      <c r="G24" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="H24" s="10" t="inlineStr"/>
       <c r="I24" s="11" t="n">
         <v>6900</v>
       </c>
@@ -5588,11 +5300,7 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B25" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B25" s="10" t="inlineStr"/>
       <c r="C25" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5608,21 +5316,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F25" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G25" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H25" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F25" s="10" t="inlineStr"/>
+      <c r="G25" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H25" s="10" t="inlineStr"/>
       <c r="I25" s="11" t="n">
         <v>8523.799999999999</v>
       </c>
@@ -5638,11 +5336,7 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B26" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B26" s="10" t="inlineStr"/>
       <c r="C26" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5658,21 +5352,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F26" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G26" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H26" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F26" s="10" t="inlineStr"/>
+      <c r="G26" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H26" s="10" t="inlineStr"/>
       <c r="I26" s="11" t="n">
         <v>7245</v>
       </c>
@@ -5688,11 +5372,7 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B27" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B27" s="10" t="inlineStr"/>
       <c r="C27" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5708,21 +5388,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F27" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G27" s="10" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="H27" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F27" s="10" t="inlineStr"/>
+      <c r="G27" s="11" t="n">
+        <v>31</v>
+      </c>
+      <c r="H27" s="10" t="inlineStr"/>
       <c r="I27" s="11" t="n">
         <v>7245</v>
       </c>
@@ -5738,11 +5408,7 @@
           <t>23:25</t>
         </is>
       </c>
-      <c r="B28" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B28" s="10" t="inlineStr"/>
       <c r="C28" s="10" t="inlineStr">
         <is>
           <t>Санкт-Петербург</t>
@@ -5758,21 +5424,11 @@
           <t>ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
-      <c r="F28" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G28" s="10" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H28" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F28" s="10" t="inlineStr"/>
+      <c r="G28" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="H28" s="10" t="inlineStr"/>
       <c r="I28" s="11" t="n">
         <v>7245</v>
       </c>
@@ -5782,175 +5438,3502 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B29" s="10" t="inlineStr"/>
+      <c r="C29" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="D29" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Международный автовокзал Саларьево</t>
+        </is>
+      </c>
+      <c r="E29" s="10" t="inlineStr">
+        <is>
+          <t>Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F29" s="10" t="inlineStr"/>
+      <c r="G29" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H29" s="10" t="inlineStr"/>
+      <c r="I29" s="11" t="n">
+        <v>2311</v>
+      </c>
+      <c r="J29" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B30" s="10" t="inlineStr"/>
+      <c r="C30" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="D30" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Международный автовокзал Северные Ворота</t>
+        </is>
+      </c>
+      <c r="E30" s="10" t="inlineStr">
+        <is>
+          <t>Круиз 21</t>
+        </is>
+      </c>
+      <c r="F30" s="10" t="inlineStr"/>
+      <c r="G30" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H30" s="10" t="inlineStr"/>
+      <c r="I30" s="11" t="n">
+        <v>2311</v>
+      </c>
+      <c r="J30" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
+      </c>
+    </row>
     <row r="31">
-      <c r="A31" s="12" t="inlineStr">
-        <is>
-          <t>Статистика</t>
-        </is>
-      </c>
-      <c r="B31" s="13" t="n"/>
+      <c r="A31" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B31" s="10" t="inlineStr"/>
+      <c r="C31" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="D31" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Автовокзал Центральный (Щелковский)</t>
+        </is>
+      </c>
+      <c r="E31" s="10" t="inlineStr">
+        <is>
+          <t>Славянский Экспресс</t>
+        </is>
+      </c>
+      <c r="F31" s="10" t="inlineStr"/>
+      <c r="G31" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H31" s="10" t="inlineStr"/>
+      <c r="I31" s="11" t="n">
+        <v>2083</v>
+      </c>
+      <c r="J31" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="inlineStr">
         <is>
-          <t>Всего рейсов</t>
-        </is>
-      </c>
-      <c r="B32" s="11" t="n">
-        <v>26</v>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B32" s="10" t="inlineStr"/>
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="D32" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Международный автовокзал Северные Ворота</t>
+        </is>
+      </c>
+      <c r="E32" s="10" t="inlineStr">
+        <is>
+          <t>Ecolines</t>
+        </is>
+      </c>
+      <c r="F32" s="10" t="inlineStr"/>
+      <c r="G32" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H32" s="10" t="inlineStr"/>
+      <c r="I32" s="11" t="n">
+        <v>2352</v>
+      </c>
+      <c r="J32" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="inlineStr">
         <is>
-          <t>Средняя цена (руб.)</t>
-        </is>
-      </c>
-      <c r="B33" s="11" t="n">
-        <v>12008.26</v>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B33" s="10" t="inlineStr"/>
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="D33" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Автовокзал Центральный (Щелковский)</t>
+        </is>
+      </c>
+      <c r="E33" s="10" t="inlineStr">
+        <is>
+          <t>Беркут</t>
+        </is>
+      </c>
+      <c r="F33" s="10" t="inlineStr"/>
+      <c r="G33" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H33" s="10" t="inlineStr"/>
+      <c r="I33" s="11" t="n">
+        <v>2197</v>
+      </c>
+      <c r="J33" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="12" t="inlineStr">
-        <is>
-          <t>Направления (Откуда)</t>
-        </is>
-      </c>
-      <c r="B34" s="13" t="n"/>
+      <c r="A34" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B34" s="10" t="inlineStr"/>
+      <c r="C34" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="D34" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Автовокзал Котельники</t>
+        </is>
+      </c>
+      <c r="E34" s="10" t="inlineStr">
+        <is>
+          <t>VolgaLine</t>
+        </is>
+      </c>
+      <c r="F34" s="10" t="inlineStr"/>
+      <c r="G34" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H34" s="10" t="inlineStr"/>
+      <c r="I34" s="11" t="n">
+        <v>2311</v>
+      </c>
+      <c r="J34" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="B35" s="11" t="n">
-        <v>26</v>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B35" s="10" t="inlineStr"/>
+      <c r="C35" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, ост. Балтийский вокзал</t>
+        </is>
+      </c>
+      <c r="D35" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Международный автовокзал Северные Ворота</t>
+        </is>
+      </c>
+      <c r="E35" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F35" s="10" t="inlineStr"/>
+      <c r="G35" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H35" s="10" t="inlineStr"/>
+      <c r="I35" s="11" t="n">
+        <v>2197</v>
+      </c>
+      <c r="J35" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="12" t="inlineStr">
-        <is>
-          <t>Прибытие (Куда)</t>
-        </is>
-      </c>
-      <c r="B36" s="13" t="n"/>
+      <c r="A36" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B36" s="10" t="inlineStr"/>
+      <c r="C36" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="D36" s="10" t="inlineStr">
+        <is>
+          <t>Москва, Международный автовокзал Саларьево</t>
+        </is>
+      </c>
+      <c r="E36" s="10" t="inlineStr">
+        <is>
+          <t>Евротранс</t>
+        </is>
+      </c>
+      <c r="F36" s="10" t="inlineStr"/>
+      <c r="G36" s="10" t="inlineStr">
+        <is>
+          <t>Есть места</t>
+        </is>
+      </c>
+      <c r="H36" s="10" t="inlineStr"/>
+      <c r="I36" s="11" t="n">
+        <v>2070</v>
+      </c>
+      <c r="J36" s="10" t="inlineStr">
+        <is>
+          <t>tutu</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Ростов-на-Дону</t>
-        </is>
-      </c>
-      <c r="B37" s="11" t="n">
-        <v>26</v>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="B37" s="10" t="inlineStr">
+        <is>
+          <t>5470</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D37" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E37" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Астория"</t>
+        </is>
+      </c>
+      <c r="F37" s="11" t="n">
+        <v>44</v>
+      </c>
+      <c r="G37" s="10" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H37" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="I37" s="11" t="n">
+        <v>2385</v>
+      </c>
+      <c r="J37" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="12" t="inlineStr">
-        <is>
-          <t>Перевозчики</t>
-        </is>
-      </c>
-      <c r="B38" s="13" t="n"/>
+      <c r="A38" s="10" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="B38" s="10" t="inlineStr">
+        <is>
+          <t>78.77.031</t>
+        </is>
+      </c>
+      <c r="C38" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D38" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E38" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F38" s="11" t="n">
+        <v>55</v>
+      </c>
+      <c r="G38" s="10" t="inlineStr">
+        <is>
+          <t>25+</t>
+        </is>
+      </c>
+      <c r="H38" s="10" t="inlineStr"/>
+      <c r="I38" s="11" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J38" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ЕвроТранс / ИП Яцунов М.С.</t>
-        </is>
-      </c>
-      <c r="B39" s="11" t="n">
-        <v>8</v>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B39" s="10" t="inlineStr">
+        <is>
+          <t>9569</t>
+        </is>
+      </c>
+      <c r="C39" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D39" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E39" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Елена Владимировна</t>
+        </is>
+      </c>
+      <c r="F39" s="11" t="n">
+        <v>53</v>
+      </c>
+      <c r="G39" s="10" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="H39" s="11" t="n">
+        <v>33</v>
+      </c>
+      <c r="I39" s="11" t="n">
+        <v>2171</v>
+      </c>
+      <c r="J39" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ФТК Сотранс</t>
-        </is>
-      </c>
-      <c r="B40" s="11" t="n">
-        <v>4</v>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B40" s="10" t="inlineStr">
+        <is>
+          <t>5192</t>
+        </is>
+      </c>
+      <c r="C40" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D40" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E40" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Славянский экспресс"</t>
+        </is>
+      </c>
+      <c r="F40" s="11" t="n">
+        <v>55</v>
+      </c>
+      <c r="G40" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H40" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="I40" s="11" t="n">
+        <v>1957</v>
+      </c>
+      <c r="J40" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Асеева Е.В.</t>
-        </is>
-      </c>
-      <c r="B41" s="11" t="n">
-        <v>4</v>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B41" s="10" t="inlineStr">
+        <is>
+          <t>5192</t>
+        </is>
+      </c>
+      <c r="C41" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D41" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E41" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Славянский экспресс"</t>
+        </is>
+      </c>
+      <c r="F41" s="11" t="n">
+        <v>55</v>
+      </c>
+      <c r="G41" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H41" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="I41" s="11" t="n">
+        <v>1957</v>
+      </c>
+      <c r="J41" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Панин Д.С.</t>
-        </is>
-      </c>
-      <c r="B42" s="11" t="n">
-        <v>2</v>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>9074</t>
+        </is>
+      </c>
+      <c r="C42" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D42" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E42" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Круиз 21"</t>
+        </is>
+      </c>
+      <c r="F42" s="11" t="n">
+        <v>51</v>
+      </c>
+      <c r="G42" s="10" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="H42" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="11" t="n">
+        <v>2171</v>
+      </c>
+      <c r="J42" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Асеева Елена Владимировна</t>
-        </is>
-      </c>
-      <c r="B43" s="11" t="n">
-        <v>2</v>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B43" s="10" t="inlineStr"/>
+      <c r="C43" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D43" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E43" s="10" t="inlineStr">
+        <is>
+          <t>ECOLINES</t>
+        </is>
+      </c>
+      <c r="F43" s="10" t="inlineStr"/>
+      <c r="G43" s="10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H43" s="10" t="inlineStr"/>
+      <c r="I43" s="11" t="n">
+        <v>2247</v>
+      </c>
+      <c r="J43" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Насиров М.М.</t>
-        </is>
-      </c>
-      <c r="B44" s="11" t="n">
-        <v>2</v>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B44" s="10" t="inlineStr">
+        <is>
+          <t>4571</t>
+        </is>
+      </c>
+      <c r="C44" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D44" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E44" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Беркут"</t>
+        </is>
+      </c>
+      <c r="F44" s="11" t="n">
+        <v>46</v>
+      </c>
+      <c r="G44" s="10" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="H44" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="I44" s="11" t="n">
+        <v>2064</v>
+      </c>
+      <c r="J44" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "АСТОРИЯ"</t>
-        </is>
-      </c>
-      <c r="B45" s="11" t="n">
-        <v>1</v>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B45" s="10" t="inlineStr">
+        <is>
+          <t>78.77.031</t>
+        </is>
+      </c>
+      <c r="C45" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D45" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E45" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F45" s="11" t="n">
+        <v>55</v>
+      </c>
+      <c r="G45" s="10" t="inlineStr">
+        <is>
+          <t>25+</t>
+        </is>
+      </c>
+      <c r="H45" s="10" t="inlineStr"/>
+      <c r="I45" s="11" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J45" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ФТК Сотранс ООО</t>
-        </is>
-      </c>
-      <c r="B46" s="11" t="n">
-        <v>1</v>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B46" s="10" t="inlineStr">
+        <is>
+          <t>4359</t>
+        </is>
+      </c>
+      <c r="C46" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D46" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E46" s="10" t="inlineStr">
+        <is>
+          <t>ООО "ВолгаЛинии"</t>
+        </is>
+      </c>
+      <c r="F46" s="11" t="n">
+        <v>46</v>
+      </c>
+      <c r="G46" s="10" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="H46" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="I46" s="11" t="n">
+        <v>2171</v>
+      </c>
+      <c r="J46" s="10" t="inlineStr">
+        <is>
+          <t>e-traffic</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Панин Дмитрий Сергеевич</t>
-        </is>
-      </c>
-      <c r="B47" s="11" t="n">
-        <v>1</v>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="B47" s="10" t="inlineStr"/>
+      <c r="C47" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D47" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E47" s="10" t="inlineStr">
+        <is>
+          <t>ООО "АСТОРИЯ"</t>
+        </is>
+      </c>
+      <c r="F47" s="10" t="inlineStr"/>
+      <c r="G47" s="10" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H47" s="10" t="inlineStr"/>
+      <c r="I47" s="11" t="n">
+        <v>4832.3</v>
+      </c>
+      <c r="J47" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="10" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="B48" s="10" t="inlineStr"/>
+      <c r="C48" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D48" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E48" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Астория"</t>
+        </is>
+      </c>
+      <c r="F48" s="10" t="inlineStr"/>
+      <c r="G48" s="10" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H48" s="10" t="inlineStr"/>
+      <c r="I48" s="11" t="n">
+        <v>2796.56</v>
+      </c>
+      <c r="J48" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B49" s="10" t="inlineStr"/>
+      <c r="C49" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D49" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E49" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Д.С.</t>
+        </is>
+      </c>
+      <c r="F49" s="10" t="inlineStr"/>
+      <c r="G49" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H49" s="10" t="inlineStr"/>
+      <c r="I49" s="11" t="n">
+        <v>14611.9</v>
+      </c>
+      <c r="J49" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B50" s="10" t="inlineStr"/>
+      <c r="C50" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D50" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E50" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Д.С.</t>
+        </is>
+      </c>
+      <c r="F50" s="10" t="inlineStr"/>
+      <c r="G50" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H50" s="10" t="inlineStr"/>
+      <c r="I50" s="11" t="n">
+        <v>14611.9</v>
+      </c>
+      <c r="J50" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B51" s="10" t="inlineStr"/>
+      <c r="C51" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D51" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E51" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Дмитрий Сергеевич</t>
+        </is>
+      </c>
+      <c r="F51" s="10" t="inlineStr"/>
+      <c r="G51" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H51" s="10" t="inlineStr"/>
+      <c r="I51" s="11" t="n">
+        <v>12420</v>
+      </c>
+      <c r="J51" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B52" s="10" t="inlineStr"/>
+      <c r="C52" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D52" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E52" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Дмитрий Сергеевич</t>
+        </is>
+      </c>
+      <c r="F52" s="10" t="inlineStr"/>
+      <c r="G52" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H52" s="10" t="inlineStr"/>
+      <c r="I52" s="11" t="n">
+        <v>12420</v>
+      </c>
+      <c r="J52" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="B53" s="10" t="inlineStr"/>
+      <c r="C53" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D53" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E53" s="10" t="inlineStr">
+        <is>
+          <t>ИП Панин Дмитрий Сергеевич</t>
+        </is>
+      </c>
+      <c r="F53" s="10" t="inlineStr"/>
+      <c r="G53" s="10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H53" s="10" t="inlineStr"/>
+      <c r="I53" s="11" t="n">
+        <v>12420</v>
+      </c>
+      <c r="J53" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B54" s="10" t="inlineStr"/>
+      <c r="C54" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D54" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E54" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F54" s="10" t="inlineStr"/>
+      <c r="G54" s="10" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="H54" s="10" t="inlineStr"/>
+      <c r="I54" s="11" t="n">
+        <v>3247.6</v>
+      </c>
+      <c r="J54" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B55" s="10" t="inlineStr"/>
+      <c r="C55" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D55" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E55" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F55" s="10" t="inlineStr"/>
+      <c r="G55" s="10" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="H55" s="10" t="inlineStr"/>
+      <c r="I55" s="11" t="n">
+        <v>2995.75</v>
+      </c>
+      <c r="J55" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B56" s="10" t="inlineStr"/>
+      <c r="C56" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D56" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E56" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Елена Владимировна</t>
+        </is>
+      </c>
+      <c r="F56" s="10" t="inlineStr"/>
+      <c r="G56" s="10" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="H56" s="10" t="inlineStr"/>
+      <c r="I56" s="11" t="n">
+        <v>2760</v>
+      </c>
+      <c r="J56" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B57" s="10" t="inlineStr"/>
+      <c r="C57" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D57" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E57" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Елена Владимировна</t>
+        </is>
+      </c>
+      <c r="F57" s="10" t="inlineStr"/>
+      <c r="G57" s="10" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="H57" s="10" t="inlineStr"/>
+      <c r="I57" s="11" t="n">
+        <v>2545.86</v>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B58" s="10" t="inlineStr"/>
+      <c r="C58" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D58" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E58" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F58" s="10" t="inlineStr"/>
+      <c r="G58" s="10" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="H58" s="10" t="inlineStr"/>
+      <c r="I58" s="11" t="n">
+        <v>3145.25</v>
+      </c>
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="10" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B59" s="10" t="inlineStr"/>
+      <c r="C59" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D59" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E59" s="10" t="inlineStr">
+        <is>
+          <t>ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="F59" s="10" t="inlineStr"/>
+      <c r="G59" s="10" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="H59" s="10" t="inlineStr"/>
+      <c r="I59" s="11" t="n">
+        <v>3409.75</v>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B60" s="10" t="inlineStr"/>
+      <c r="C60" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D60" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E60" s="10" t="inlineStr"/>
+      <c r="F60" s="10" t="inlineStr"/>
+      <c r="G60" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H60" s="10" t="inlineStr"/>
+      <c r="I60" s="11" t="n">
+        <v>2700.2</v>
+      </c>
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B61" s="10" t="inlineStr"/>
+      <c r="C61" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D61" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E61" s="10" t="inlineStr"/>
+      <c r="F61" s="10" t="inlineStr"/>
+      <c r="G61" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H61" s="10" t="inlineStr"/>
+      <c r="I61" s="11" t="n">
+        <v>2700.2</v>
+      </c>
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B62" s="10" t="inlineStr"/>
+      <c r="C62" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D62" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E62" s="10" t="inlineStr">
+        <is>
+          <t>ООО "СЛАВЯНСКИЙ ЭКСПРЕСС"</t>
+        </is>
+      </c>
+      <c r="F62" s="10" t="inlineStr"/>
+      <c r="G62" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H62" s="10" t="inlineStr"/>
+      <c r="I62" s="11" t="n">
+        <v>2295.16</v>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B63" s="10" t="inlineStr"/>
+      <c r="C63" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D63" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E63" s="10" t="inlineStr">
+        <is>
+          <t>ООО "СЛАВЯНСКИЙ ЭКСПРЕСС"</t>
+        </is>
+      </c>
+      <c r="F63" s="10" t="inlineStr"/>
+      <c r="G63" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H63" s="10" t="inlineStr"/>
+      <c r="I63" s="11" t="n">
+        <v>2295.16</v>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B64" s="10" t="inlineStr"/>
+      <c r="C64" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D64" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E64" s="10" t="inlineStr">
+        <is>
+          <t>ООО "Круиз 21"</t>
+        </is>
+      </c>
+      <c r="F64" s="10" t="inlineStr"/>
+      <c r="G64" s="10" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="H64" s="10" t="inlineStr"/>
+      <c r="I64" s="11" t="n">
+        <v>2335.65</v>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B65" s="10" t="inlineStr"/>
+      <c r="C65" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D65" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E65" s="10" t="inlineStr"/>
+      <c r="F65" s="10" t="inlineStr"/>
+      <c r="G65" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H65" s="10" t="inlineStr"/>
+      <c r="I65" s="11" t="n">
+        <v>2834.75</v>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="10" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="B66" s="10" t="inlineStr"/>
+      <c r="C66" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D66" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E66" s="10" t="inlineStr"/>
+      <c r="F66" s="10" t="inlineStr"/>
+      <c r="G66" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H66" s="10" t="inlineStr"/>
+      <c r="I66" s="11" t="n">
+        <v>2834.75</v>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B67" s="10" t="inlineStr"/>
+      <c r="C67" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D67" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E67" s="10" t="inlineStr"/>
+      <c r="F67" s="10" t="inlineStr"/>
+      <c r="G67" s="10" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="H67" s="10" t="inlineStr"/>
+      <c r="I67" s="11" t="n">
+        <v>3040.6</v>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B68" s="10" t="inlineStr"/>
+      <c r="C68" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D68" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E68" s="10" t="inlineStr"/>
+      <c r="F68" s="10" t="inlineStr"/>
+      <c r="G68" s="10" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="H68" s="10" t="inlineStr"/>
+      <c r="I68" s="11" t="n">
+        <v>2983.1</v>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B69" s="10" t="inlineStr"/>
+      <c r="C69" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D69" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E69" s="10" t="inlineStr"/>
+      <c r="F69" s="10" t="inlineStr"/>
+      <c r="G69" s="10" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="H69" s="10" t="inlineStr"/>
+      <c r="I69" s="11" t="n">
+        <v>2535.75</v>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B70" s="10" t="inlineStr"/>
+      <c r="C70" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D70" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E70" s="10" t="inlineStr"/>
+      <c r="F70" s="10" t="inlineStr"/>
+      <c r="G70" s="10" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="H70" s="10" t="inlineStr"/>
+      <c r="I70" s="11" t="n">
+        <v>3192.4</v>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="10" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="B71" s="10" t="inlineStr"/>
+      <c r="C71" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D71" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E71" s="10" t="inlineStr"/>
+      <c r="F71" s="10" t="inlineStr"/>
+      <c r="G71" s="10" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="H71" s="10" t="inlineStr"/>
+      <c r="I71" s="11" t="n">
+        <v>3132.6</v>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="10" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B72" s="10" t="inlineStr"/>
+      <c r="C72" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D72" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E72" s="10" t="inlineStr"/>
+      <c r="F72" s="10" t="inlineStr"/>
+      <c r="G72" s="10" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="H72" s="10" t="inlineStr"/>
+      <c r="I72" s="11" t="n">
+        <v>2847.4</v>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="10" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B73" s="10" t="inlineStr"/>
+      <c r="C73" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D73" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E73" s="10" t="inlineStr">
+        <is>
+          <t>ООО "БЕРКУТ"</t>
+        </is>
+      </c>
+      <c r="F73" s="10" t="inlineStr"/>
+      <c r="G73" s="10" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="H73" s="10" t="inlineStr"/>
+      <c r="I73" s="11" t="n">
+        <v>2420.51</v>
+      </c>
+      <c r="J73" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="10" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="B74" s="10" t="inlineStr"/>
+      <c r="C74" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D74" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E74" s="10" t="inlineStr"/>
+      <c r="F74" s="10" t="inlineStr"/>
+      <c r="G74" s="10" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="H74" s="10" t="inlineStr"/>
+      <c r="I74" s="11" t="n">
+        <v>2990</v>
+      </c>
+      <c r="J74" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B75" s="10" t="inlineStr"/>
+      <c r="C75" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D75" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E75" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F75" s="10" t="inlineStr"/>
+      <c r="G75" s="10" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="H75" s="10" t="inlineStr"/>
+      <c r="I75" s="11" t="n">
+        <v>2185</v>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B76" s="10" t="inlineStr"/>
+      <c r="C76" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D76" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E76" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="F76" s="10" t="inlineStr"/>
+      <c r="G76" s="10" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="H76" s="10" t="inlineStr"/>
+      <c r="I76" s="11" t="n">
+        <v>2570.25</v>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B77" s="10" t="inlineStr"/>
+      <c r="C77" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D77" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E77" s="10" t="inlineStr"/>
+      <c r="F77" s="10" t="inlineStr"/>
+      <c r="G77" s="10" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr"/>
+      <c r="I77" s="11" t="n">
+        <v>2435.7</v>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B78" s="10" t="inlineStr"/>
+      <c r="C78" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D78" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E78" s="10" t="inlineStr"/>
+      <c r="F78" s="10" t="inlineStr"/>
+      <c r="G78" s="10" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr"/>
+      <c r="I78" s="11" t="n">
+        <v>2922.15</v>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B79" s="10" t="inlineStr"/>
+      <c r="C79" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D79" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E79" s="10" t="inlineStr"/>
+      <c r="F79" s="10" t="inlineStr"/>
+      <c r="G79" s="10" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr"/>
+      <c r="I79" s="11" t="n">
+        <v>2995.75</v>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B80" s="10" t="inlineStr"/>
+      <c r="C80" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D80" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E80" s="10" t="inlineStr"/>
+      <c r="F80" s="10" t="inlineStr"/>
+      <c r="G80" s="10" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr"/>
+      <c r="I80" s="11" t="n">
+        <v>2484</v>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B81" s="10" t="inlineStr"/>
+      <c r="C81" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D81" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E81" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F81" s="10" t="inlineStr"/>
+      <c r="G81" s="10" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr"/>
+      <c r="I81" s="11" t="n">
+        <v>2648.45</v>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B82" s="10" t="inlineStr"/>
+      <c r="C82" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D82" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E82" s="10" t="inlineStr">
+        <is>
+          <t>ООО "ВОЛГАЛИНИИ"</t>
+        </is>
+      </c>
+      <c r="F82" s="10" t="inlineStr"/>
+      <c r="G82" s="10" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr"/>
+      <c r="I82" s="11" t="n">
+        <v>2545.86</v>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B83" s="10" t="inlineStr"/>
+      <c r="C83" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D83" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E83" s="10" t="inlineStr">
+        <is>
+          <t>ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="F83" s="10" t="inlineStr"/>
+      <c r="G83" s="10" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr"/>
+      <c r="I83" s="11" t="n">
+        <v>2185</v>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B84" s="10" t="inlineStr"/>
+      <c r="C84" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D84" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E84" s="10" t="inlineStr">
+        <is>
+          <t>ООО "ВОЛГАЛИНИИ"</t>
+        </is>
+      </c>
+      <c r="F84" s="10" t="inlineStr"/>
+      <c r="G84" s="10" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr"/>
+      <c r="I84" s="11" t="n">
+        <v>2070</v>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B85" s="10" t="inlineStr"/>
+      <c r="C85" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D85" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E85" s="10" t="inlineStr"/>
+      <c r="F85" s="10" t="inlineStr"/>
+      <c r="G85" s="10" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr"/>
+      <c r="I85" s="11" t="n">
+        <v>2557.6</v>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B86" s="10" t="inlineStr"/>
+      <c r="C86" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D86" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E86" s="10" t="inlineStr"/>
+      <c r="F86" s="10" t="inlineStr"/>
+      <c r="G86" s="10" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr"/>
+      <c r="I86" s="11" t="n">
+        <v>3068.2</v>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="10" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="B87" s="10" t="inlineStr"/>
+      <c r="C87" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D87" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E87" s="10" t="inlineStr"/>
+      <c r="F87" s="10" t="inlineStr"/>
+      <c r="G87" s="10" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr"/>
+      <c r="I87" s="11" t="n">
+        <v>3145.25</v>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B88" s="10" t="inlineStr"/>
+      <c r="C88" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D88" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E88" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F88" s="10" t="inlineStr"/>
+      <c r="G88" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr"/>
+      <c r="I88" s="11" t="n">
+        <v>2300</v>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B89" s="10" t="inlineStr"/>
+      <c r="C89" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D89" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E89" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F89" s="10" t="inlineStr"/>
+      <c r="G89" s="10" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr"/>
+      <c r="I89" s="11" t="n">
+        <v>2705.95</v>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B90" s="10" t="inlineStr"/>
+      <c r="C90" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D90" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E90" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс (ИП Яцунов С.П.)</t>
+        </is>
+      </c>
+      <c r="F90" s="10" t="inlineStr"/>
+      <c r="G90" s="10" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr"/>
+      <c r="I90" s="11" t="n">
+        <v>2760</v>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B91" s="10" t="inlineStr"/>
+      <c r="C91" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D91" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E91" s="10" t="inlineStr">
+        <is>
+          <t>ИП Яцунов Максим Сергеевич</t>
+        </is>
+      </c>
+      <c r="F91" s="10" t="inlineStr"/>
+      <c r="G91" s="10" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr"/>
+      <c r="I91" s="11" t="n">
+        <v>2300</v>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B92" s="10" t="inlineStr"/>
+      <c r="C92" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D92" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E92" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F92" s="10" t="inlineStr"/>
+      <c r="G92" s="10" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr"/>
+      <c r="I92" s="11" t="n">
+        <v>2841.65</v>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="10" t="inlineStr">
+        <is>
+          <t>23:25</t>
+        </is>
+      </c>
+      <c r="B93" s="10" t="inlineStr"/>
+      <c r="C93" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D93" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E93" s="10" t="inlineStr">
+        <is>
+          <t>ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="F93" s="10" t="inlineStr"/>
+      <c r="G93" s="10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr"/>
+      <c r="I93" s="11" t="n">
+        <v>2415</v>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>avtovokzalspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="10" t="inlineStr">
+        <is>
+          <t>23:25
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B94" s="10" t="inlineStr"/>
+      <c r="C94" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D94" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E94" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F94" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G94" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H94" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I94" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J94" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="10" t="inlineStr">
+        <is>
+          <t>23:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B95" s="10" t="inlineStr"/>
+      <c r="C95" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D95" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E95" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F95" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G95" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H95" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I95" s="11" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J95" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="10" t="inlineStr">
+        <is>
+          <t>23:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B96" s="10" t="inlineStr"/>
+      <c r="C96" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D96" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E96" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F96" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G96" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H96" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I96" s="11" t="n">
+        <v>1944</v>
+      </c>
+      <c r="J96" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="10" t="inlineStr">
+        <is>
+          <t>20:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B97" s="10" t="inlineStr"/>
+      <c r="C97" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D97" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E97" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F97" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G97" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H97" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I97" s="11" t="n">
+        <v>1996</v>
+      </c>
+      <c r="J97" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="10" t="inlineStr">
+        <is>
+          <t>20:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B98" s="10" t="inlineStr"/>
+      <c r="C98" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D98" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E98" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F98" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G98" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H98" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I98" s="11" t="n">
+        <v>1996</v>
+      </c>
+      <c r="J98" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="10" t="inlineStr">
+        <is>
+          <t>23:25
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B99" s="10" t="inlineStr"/>
+      <c r="C99" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D99" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E99" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F99" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G99" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H99" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I99" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J99" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="10" t="inlineStr">
+        <is>
+          <t>22:30
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B100" s="10" t="inlineStr"/>
+      <c r="C100" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D100" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E100" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F100" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G100" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H100" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I100" s="11" t="n">
+        <v>2105</v>
+      </c>
+      <c r="J100" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="10" t="inlineStr">
+        <is>
+          <t>20:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B101" s="10" t="inlineStr"/>
+      <c r="C101" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D101" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E101" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F101" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G101" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H101" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I101" s="11" t="n">
+        <v>2133</v>
+      </c>
+      <c r="J101" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="10" t="inlineStr">
+        <is>
+          <t>21:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B102" s="10" t="inlineStr"/>
+      <c r="C102" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D102" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E102" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F102" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G102" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H102" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I102" s="11" t="n">
+        <v>2195</v>
+      </c>
+      <c r="J102" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="10" t="inlineStr">
+        <is>
+          <t>23:25
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B103" s="10" t="inlineStr"/>
+      <c r="C103" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D103" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E103" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F103" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G103" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H103" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I103" s="11" t="n">
+        <v>2200</v>
+      </c>
+      <c r="J103" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="10" t="inlineStr">
+        <is>
+          <t>17:30
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B104" s="10" t="inlineStr"/>
+      <c r="C104" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D104" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E104" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F104" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G104" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H104" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I104" s="11" t="n">
+        <v>2214</v>
+      </c>
+      <c r="J104" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="10" t="inlineStr">
+        <is>
+          <t>23:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B105" s="10" t="inlineStr"/>
+      <c r="C105" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D105" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E105" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F105" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G105" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H105" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I105" s="11" t="n">
+        <v>2214</v>
+      </c>
+      <c r="J105" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="10" t="inlineStr">
+        <is>
+          <t>10:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B106" s="10" t="inlineStr"/>
+      <c r="C106" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D106" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E106" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F106" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G106" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H106" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I106" s="11" t="n">
+        <v>2432</v>
+      </c>
+      <c r="J106" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="12" t="inlineStr">
+        <is>
+          <t>Статистика</t>
+        </is>
+      </c>
+      <c r="B109" s="13" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="10" t="inlineStr">
+        <is>
+          <t>Всего рейсов</t>
+        </is>
+      </c>
+      <c r="B110" s="11" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="10" t="inlineStr">
+        <is>
+          <t>Средняя цена (руб.)</t>
+        </is>
+      </c>
+      <c r="B111" s="11" t="n">
+        <v>5392.21</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="12" t="inlineStr">
+        <is>
+          <t>Направления (Откуда)</t>
+        </is>
+      </c>
+      <c r="B112" s="13" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="B113" s="11" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Санкт-Петербург, Автовокзал</t>
+        </is>
+      </c>
+      <c r="B114" s="11" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Санкт-Петербург, ост. Балтийский вокзал</t>
+        </is>
+      </c>
+      <c r="B115" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="12" t="inlineStr">
+        <is>
+          <t>Прибытие (Куда)</t>
+        </is>
+      </c>
+      <c r="B116" s="13" t="n"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Москва</t>
+        </is>
+      </c>
+      <c r="B117" s="11" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="B118" s="11" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Москва, Международный автовокзал Северные Ворота</t>
+        </is>
+      </c>
+      <c r="B119" s="11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Москва, Международный автовокзал Саларьево</t>
+        </is>
+      </c>
+      <c r="B120" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Москва, Автовокзал Центральный (Щелковский)</t>
+        </is>
+      </c>
+      <c r="B121" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Москва, Автовокзал Котельники</t>
+        </is>
+      </c>
+      <c r="B122" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="12" t="inlineStr">
+        <is>
+          <t>Перевозчики</t>
+        </is>
+      </c>
+      <c r="B123" s="13" t="n"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ЕвроТранс / ИП Яцунов М.С.</t>
+        </is>
+      </c>
+      <c r="B124" s="11" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="B125" s="11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ФТК Сотранс</t>
+        </is>
+      </c>
+      <c r="B126" s="11" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ФТК Сотранс ООО</t>
+        </is>
+      </c>
+      <c r="B127" s="11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Асеева Елена Владимировна</t>
+        </is>
+      </c>
+      <c r="B128" s="11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Панин Д.С.</t>
+        </is>
+      </c>
+      <c r="B129" s="11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Панин Дмитрий Сергеевич</t>
+        </is>
+      </c>
+      <c r="B130" s="11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "ВОЛГАЛИНИИ"</t>
+        </is>
+      </c>
+      <c r="B131" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "СЛАВЯНСКИЙ ЭКСПРЕСС"</t>
+        </is>
+      </c>
+      <c r="B132" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "Круиз 21"</t>
+        </is>
+      </c>
+      <c r="B133" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "Славянский экспресс"</t>
+        </is>
+      </c>
+      <c r="B134" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "Астория"</t>
+        </is>
+      </c>
+      <c r="B135" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "АСТОРИЯ"</t>
+        </is>
+      </c>
+      <c r="B136" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Насиров М.М.</t>
+        </is>
+      </c>
+      <c r="B137" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Ecolines</t>
+        </is>
+      </c>
+      <c r="B138" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  VolgaLine</t>
+        </is>
+      </c>
+      <c r="B139" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Евротранс</t>
+        </is>
+      </c>
+      <c r="B140" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Славянский Экспресс</t>
+        </is>
+      </c>
+      <c r="B141" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Круиз 21</t>
+        </is>
+      </c>
+      <c r="B142" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="B143" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ECOLINES</t>
+        </is>
+      </c>
+      <c r="B144" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "Беркут"</t>
+        </is>
+      </c>
+      <c r="B145" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "ВолгаЛинии"</t>
+        </is>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "БЕРКУТ"</t>
+        </is>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="10" t="inlineStr">
+        <is>
           <t xml:space="preserve">  ИП Насиров Махир Музаффар Оглы</t>
         </is>
       </c>
-      <c r="B48" s="11" t="n">
+      <c r="B148" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ЕвроТранс (ИП Яцунов С.П.)</t>
+        </is>
+      </c>
+      <c r="B149" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Яцунов Максим Сергеевич</t>
+        </is>
+      </c>
+      <c r="B150" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Беркут</t>
+        </is>
+      </c>
+      <c r="B151" s="11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
busfor, e-traffic, словарь городов, tutu, avtovokzal, selenium2
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -4398,7 +4398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7927,21 +7927,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F94" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F94" s="10" t="inlineStr"/>
       <c r="G94" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H94" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H94" s="10" t="inlineStr"/>
       <c r="I94" s="11" t="n">
         <v>2000</v>
       </c>
@@ -7974,21 +7966,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F95" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F95" s="10" t="inlineStr"/>
       <c r="G95" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H95" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H95" s="10" t="inlineStr"/>
       <c r="I95" s="11" t="n">
         <v>1900</v>
       </c>
@@ -8021,21 +8005,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F96" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F96" s="10" t="inlineStr"/>
       <c r="G96" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H96" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H96" s="10" t="inlineStr"/>
       <c r="I96" s="11" t="n">
         <v>1944</v>
       </c>
@@ -8068,21 +8044,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F97" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F97" s="10" t="inlineStr"/>
       <c r="G97" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H97" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H97" s="10" t="inlineStr"/>
       <c r="I97" s="11" t="n">
         <v>1996</v>
       </c>
@@ -8115,21 +8083,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F98" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F98" s="10" t="inlineStr"/>
       <c r="G98" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H98" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H98" s="10" t="inlineStr"/>
       <c r="I98" s="11" t="n">
         <v>1996</v>
       </c>
@@ -8162,21 +8122,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F99" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F99" s="10" t="inlineStr"/>
       <c r="G99" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H99" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H99" s="10" t="inlineStr"/>
       <c r="I99" s="11" t="n">
         <v>2000</v>
       </c>
@@ -8209,21 +8161,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F100" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F100" s="10" t="inlineStr"/>
       <c r="G100" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H100" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H100" s="10" t="inlineStr"/>
       <c r="I100" s="11" t="n">
         <v>2105</v>
       </c>
@@ -8256,21 +8200,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F101" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F101" s="10" t="inlineStr"/>
       <c r="G101" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H101" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H101" s="10" t="inlineStr"/>
       <c r="I101" s="11" t="n">
         <v>2133</v>
       </c>
@@ -8303,21 +8239,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F102" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F102" s="10" t="inlineStr"/>
       <c r="G102" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H102" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H102" s="10" t="inlineStr"/>
       <c r="I102" s="11" t="n">
         <v>2195</v>
       </c>
@@ -8350,21 +8278,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F103" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F103" s="10" t="inlineStr"/>
       <c r="G103" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H103" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H103" s="10" t="inlineStr"/>
       <c r="I103" s="11" t="n">
         <v>2200</v>
       </c>
@@ -8397,21 +8317,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F104" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F104" s="10" t="inlineStr"/>
       <c r="G104" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H104" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H104" s="10" t="inlineStr"/>
       <c r="I104" s="11" t="n">
         <v>2214</v>
       </c>
@@ -8444,21 +8356,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F105" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F105" s="10" t="inlineStr"/>
       <c r="G105" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H105" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H105" s="10" t="inlineStr"/>
       <c r="I105" s="11" t="n">
         <v>2214</v>
       </c>
@@ -8491,21 +8395,13 @@
           <t>Не определен</t>
         </is>
       </c>
-      <c r="F106" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F106" s="10" t="inlineStr"/>
       <c r="G106" s="10" t="inlineStr">
         <is>
           <t>10+</t>
         </is>
       </c>
-      <c r="H106" s="10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H106" s="10" t="inlineStr"/>
       <c r="I106" s="11" t="n">
         <v>2432</v>
       </c>
@@ -8515,242 +8411,725 @@
         </is>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" s="10" t="inlineStr">
+        <is>
+          <t>23:25
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B107" s="10" t="inlineStr"/>
+      <c r="C107" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D107" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E107" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F107" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G107" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H107" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I107" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J107" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="10" t="inlineStr">
+        <is>
+          <t>23:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B108" s="10" t="inlineStr"/>
+      <c r="C108" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D108" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E108" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F108" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G108" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H108" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I108" s="11" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J108" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
+    </row>
     <row r="109">
-      <c r="A109" s="12" t="inlineStr">
-        <is>
-          <t>Статистика</t>
-        </is>
-      </c>
-      <c r="B109" s="13" t="n"/>
+      <c r="A109" s="10" t="inlineStr">
+        <is>
+          <t>23:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B109" s="10" t="inlineStr"/>
+      <c r="C109" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D109" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E109" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F109" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G109" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H109" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I109" s="11" t="n">
+        <v>1944</v>
+      </c>
+      <c r="J109" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="10" t="inlineStr">
         <is>
-          <t>Всего рейсов</t>
-        </is>
-      </c>
-      <c r="B110" s="11" t="n">
-        <v>104</v>
+          <t>20:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B110" s="10" t="inlineStr"/>
+      <c r="C110" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D110" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E110" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F110" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G110" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H110" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I110" s="11" t="n">
+        <v>1996</v>
+      </c>
+      <c r="J110" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="10" t="inlineStr">
         <is>
-          <t>Средняя цена (руб.)</t>
-        </is>
-      </c>
-      <c r="B111" s="11" t="n">
-        <v>5392.21</v>
+          <t>20:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B111" s="10" t="inlineStr"/>
+      <c r="C111" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D111" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E111" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F111" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G111" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H111" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I111" s="11" t="n">
+        <v>1996</v>
+      </c>
+      <c r="J111" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="12" t="inlineStr">
-        <is>
-          <t>Направления (Откуда)</t>
-        </is>
-      </c>
-      <c r="B112" s="13" t="n"/>
+      <c r="A112" s="10" t="inlineStr">
+        <is>
+          <t>23:25
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B112" s="10" t="inlineStr"/>
+      <c r="C112" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D112" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E112" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F112" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G112" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H112" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I112" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J112" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="B113" s="11" t="n">
-        <v>96</v>
+          <t>22:30
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B113" s="10" t="inlineStr"/>
+      <c r="C113" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D113" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E113" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F113" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G113" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H113" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I113" s="11" t="n">
+        <v>2105</v>
+      </c>
+      <c r="J113" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Санкт-Петербург, Автовокзал</t>
-        </is>
-      </c>
-      <c r="B114" s="11" t="n">
-        <v>7</v>
+          <t>20:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B114" s="10" t="inlineStr"/>
+      <c r="C114" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D114" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E114" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F114" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G114" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H114" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I114" s="11" t="n">
+        <v>2133</v>
+      </c>
+      <c r="J114" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Санкт-Петербург, ост. Балтийский вокзал</t>
-        </is>
-      </c>
-      <c r="B115" s="11" t="n">
-        <v>1</v>
+          <t>21:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B115" s="10" t="inlineStr"/>
+      <c r="C115" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D115" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E115" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F115" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G115" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H115" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I115" s="11" t="n">
+        <v>2195</v>
+      </c>
+      <c r="J115" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="12" t="inlineStr">
-        <is>
-          <t>Прибытие (Куда)</t>
-        </is>
-      </c>
-      <c r="B116" s="13" t="n"/>
+      <c r="A116" s="10" t="inlineStr">
+        <is>
+          <t>23:25
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B116" s="10" t="inlineStr"/>
+      <c r="C116" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D116" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E116" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F116" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G116" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H116" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I116" s="11" t="n">
+        <v>2200</v>
+      </c>
+      <c r="J116" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Москва</t>
-        </is>
-      </c>
-      <c r="B117" s="11" t="n">
-        <v>70</v>
+          <t>17:30
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B117" s="10" t="inlineStr"/>
+      <c r="C117" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D117" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E117" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F117" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G117" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H117" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I117" s="11" t="n">
+        <v>2214</v>
+      </c>
+      <c r="J117" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Ростов-на-Дону</t>
-        </is>
-      </c>
-      <c r="B118" s="11" t="n">
-        <v>26</v>
+          <t>23:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B118" s="10" t="inlineStr"/>
+      <c r="C118" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D118" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E118" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F118" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G118" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H118" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I118" s="11" t="n">
+        <v>2214</v>
+      </c>
+      <c r="J118" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Москва, Международный автовокзал Северные Ворота</t>
-        </is>
-      </c>
-      <c r="B119" s="11" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Москва, Международный автовокзал Саларьево</t>
-        </is>
-      </c>
-      <c r="B120" s="11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Москва, Автовокзал Центральный (Щелковский)</t>
-        </is>
-      </c>
-      <c r="B121" s="11" t="n">
-        <v>2</v>
+          <t>10:00
+12 авг.</t>
+        </is>
+      </c>
+      <c r="B119" s="10" t="inlineStr"/>
+      <c r="C119" s="10" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D119" s="10" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E119" s="10" t="inlineStr">
+        <is>
+          <t>Не определен</t>
+        </is>
+      </c>
+      <c r="F119" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G119" s="10" t="inlineStr">
+        <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="H119" s="10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I119" s="11" t="n">
+        <v>2432</v>
+      </c>
+      <c r="J119" s="10" t="inlineStr">
+        <is>
+          <t>busfor</t>
+        </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Москва, Автовокзал Котельники</t>
-        </is>
-      </c>
-      <c r="B122" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="A122" s="12" t="inlineStr">
+        <is>
+          <t>Статистика</t>
+        </is>
+      </c>
+      <c r="B122" s="13" t="n"/>
     </row>
     <row r="123">
-      <c r="A123" s="12" t="inlineStr">
-        <is>
-          <t>Перевозчики</t>
-        </is>
-      </c>
-      <c r="B123" s="13" t="n"/>
+      <c r="A123" s="10" t="inlineStr">
+        <is>
+          <t>Всего рейсов</t>
+        </is>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>117</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ЕвроТранс / ИП Яцунов М.С.</t>
+          <t>Средняя цена (руб.)</t>
         </is>
       </c>
       <c r="B124" s="11" t="n">
-        <v>12</v>
+        <v>5026.65</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  ИП Асеева Е.В.</t>
-        </is>
-      </c>
-      <c r="B125" s="11" t="n">
-        <v>8</v>
-      </c>
+      <c r="A125" s="12" t="inlineStr">
+        <is>
+          <t>Направления (Откуда)</t>
+        </is>
+      </c>
+      <c r="B125" s="13" t="n"/>
     </row>
     <row r="126">
       <c r="A126" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ФТК Сотранс</t>
+          <t xml:space="preserve">  Санкт-Петербург</t>
         </is>
       </c>
       <c r="B126" s="11" t="n">
-        <v>7</v>
+        <v>109</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ФТК Сотранс ООО</t>
+          <t xml:space="preserve">  Санкт-Петербург, Автовокзал</t>
         </is>
       </c>
       <c r="B127" s="11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Асеева Елена Владимировна</t>
+          <t xml:space="preserve">  Санкт-Петербург, ост. Балтийский вокзал</t>
         </is>
       </c>
       <c r="B128" s="11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  ИП Панин Д.С.</t>
-        </is>
-      </c>
-      <c r="B129" s="11" t="n">
-        <v>4</v>
-      </c>
+      <c r="A129" s="12" t="inlineStr">
+        <is>
+          <t>Прибытие (Куда)</t>
+        </is>
+      </c>
+      <c r="B129" s="13" t="n"/>
     </row>
     <row r="130">
       <c r="A130" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Панин Дмитрий Сергеевич</t>
+          <t xml:space="preserve">  Москва</t>
         </is>
       </c>
       <c r="B130" s="11" t="n">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "ВОЛГАЛИНИИ"</t>
+          <t xml:space="preserve">  Ростов-на-Дону</t>
         </is>
       </c>
       <c r="B131" s="11" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "СЛАВЯНСКИЙ ЭКСПРЕСС"</t>
+          <t xml:space="preserve">  Москва, Международный автовокзал Северные Ворота</t>
         </is>
       </c>
       <c r="B132" s="11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "Круиз 21"</t>
+          <t xml:space="preserve">  Москва, Международный автовокзал Саларьево</t>
         </is>
       </c>
       <c r="B133" s="11" t="n">
@@ -8760,7 +9139,7 @@
     <row r="134">
       <c r="A134" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "Славянский экспресс"</t>
+          <t xml:space="preserve">  Москва, Автовокзал Центральный (Щелковский)</t>
         </is>
       </c>
       <c r="B134" s="11" t="n">
@@ -8770,170 +9149,298 @@
     <row r="135">
       <c r="A135" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "Астория"</t>
+          <t xml:space="preserve">  Москва, Автовокзал Котельники</t>
         </is>
       </c>
       <c r="B135" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  ООО "АСТОРИЯ"</t>
-        </is>
-      </c>
-      <c r="B136" s="11" t="n">
-        <v>2</v>
-      </c>
+      <c r="A136" s="12" t="inlineStr">
+        <is>
+          <t>Перевозчики</t>
+        </is>
+      </c>
+      <c r="B136" s="13" t="n"/>
     </row>
     <row r="137">
       <c r="A137" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Насиров М.М.</t>
+          <t xml:space="preserve">  ЕвроТранс / ИП Яцунов М.С.</t>
         </is>
       </c>
       <c r="B137" s="11" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Ecolines</t>
+          <t xml:space="preserve">  ИП Асеева Е.В.</t>
         </is>
       </c>
       <c r="B138" s="11" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  VolgaLine</t>
+          <t xml:space="preserve">  ФТК Сотранс</t>
         </is>
       </c>
       <c r="B139" s="11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Евротранс</t>
+          <t xml:space="preserve">  ФТК Сотранс ООО</t>
         </is>
       </c>
       <c r="B140" s="11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Славянский Экспресс</t>
+          <t xml:space="preserve">  ИП Асеева Елена Владимировна</t>
         </is>
       </c>
       <c r="B141" s="11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Круиз 21</t>
+          <t xml:space="preserve">  ИП Панин Д.С.</t>
         </is>
       </c>
       <c r="B142" s="11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Асеева Е.В.</t>
+          <t xml:space="preserve">  ИП Панин Дмитрий Сергеевич</t>
         </is>
       </c>
       <c r="B143" s="11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ECOLINES</t>
+          <t xml:space="preserve">  ООО "ВОЛГАЛИНИИ"</t>
         </is>
       </c>
       <c r="B144" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "Беркут"</t>
+          <t xml:space="preserve">  ООО "СЛАВЯНСКИЙ ЭКСПРЕСС"</t>
         </is>
       </c>
       <c r="B145" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "ВолгаЛинии"</t>
+          <t xml:space="preserve">  ООО "Круиз 21"</t>
         </is>
       </c>
       <c r="B146" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ООО "БЕРКУТ"</t>
+          <t xml:space="preserve">  ООО "Славянский экспресс"</t>
         </is>
       </c>
       <c r="B147" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Насиров Махир Музаффар Оглы</t>
+          <t xml:space="preserve">  ООО "Астория"</t>
         </is>
       </c>
       <c r="B148" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ЕвроТранс (ИП Яцунов С.П.)</t>
+          <t xml:space="preserve">  ООО "АСТОРИЯ"</t>
         </is>
       </c>
       <c r="B149" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  ИП Яцунов Максим Сергеевич</t>
+          <t xml:space="preserve">  ИП Насиров М.М.</t>
         </is>
       </c>
       <c r="B150" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="10" t="inlineStr">
         <is>
+          <t xml:space="preserve">  Ecolines</t>
+        </is>
+      </c>
+      <c r="B151" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  VolgaLine</t>
+        </is>
+      </c>
+      <c r="B152" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Евротранс</t>
+        </is>
+      </c>
+      <c r="B153" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Славянский Экспресс</t>
+        </is>
+      </c>
+      <c r="B154" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Круиз 21</t>
+        </is>
+      </c>
+      <c r="B155" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Асеева Е.В.</t>
+        </is>
+      </c>
+      <c r="B156" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ECOLINES</t>
+        </is>
+      </c>
+      <c r="B157" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "Беркут"</t>
+        </is>
+      </c>
+      <c r="B158" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "ВолгаЛинии"</t>
+        </is>
+      </c>
+      <c r="B159" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ООО "БЕРКУТ"</t>
+        </is>
+      </c>
+      <c r="B160" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Насиров Махир Музаффар Оглы</t>
+        </is>
+      </c>
+      <c r="B161" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ЕвроТранс (ИП Яцунов С.П.)</t>
+        </is>
+      </c>
+      <c r="B162" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ИП Яцунов Максим Сергеевич</t>
+        </is>
+      </c>
+      <c r="B163" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="10" t="inlineStr">
+        <is>
           <t xml:space="preserve">  Беркут</t>
         </is>
       </c>
-      <c r="B151" s="11" t="n">
+      <c r="B164" s="11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>